<commit_message>
Last version for the course
Non-ready table which should've been shown only when a particular selection from dropdown was selected.
</commit_message>
<xml_diff>
--- a/assets/tables/kalat.xlsx
+++ b/assets/tables/kalat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tatu\Desktop\web-sovellukset\Web-sovellukset-lopputy-\assets\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D857B9-88ED-427A-9F1A-5D9BFFEF0485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546E8306-9F1C-4653-A5A6-1B50167C29B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>tatu</t>
   </si>
@@ -33,7 +33,10 @@
     <t>harri</t>
   </si>
   <si>
-    <t>ahti</t>
+    <t>samuli</t>
+  </si>
+  <si>
+    <t>markus</t>
   </si>
 </sst>
 </file>
@@ -351,27 +354,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>